<commit_message>
Stage 1 of incorporating admin
</commit_message>
<xml_diff>
--- a/FOMS/data/staff_list.xlsx
+++ b/FOMS/data/staff_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3919CA1E-2F3D-4B78-8D06-E0C4CD030FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD78298-2F77-4BBD-8ECB-C29EA59F8557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>ec084e54-155c-4a11-b8e8-04df6cfe3c87</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>244e4090-f72c-4ef3-8817-0f88efcf78ed</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
 </sst>
 </file>
@@ -558,13 +573,13 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -594,10 +609,10 @@
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -606,8 +621,8 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>32</v>
+      <c r="F2" t="s">
+        <v>36</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -752,8 +767,27 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>

</xml_diff>

<commit_message>
Admin editing staff accounts works
</commit_message>
<xml_diff>
--- a/FOMS/data/staff_list.xlsx
+++ b/FOMS/data/staff_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\SC2002_OOP_FOMS\FOMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD78298-2F77-4BBD-8ECB-C29EA59F8557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B4B587-DD56-4E72-82B9-B5108D6C0E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -142,16 +142,43 @@
     <t>33</t>
   </si>
   <si>
-    <t>244e4090-f72c-4ef3-8817-0f88efcf78ed</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>tester</t>
-  </si>
-  <si>
     <t>43</t>
+  </si>
+  <si>
+    <t>90b56832-f283-491f-86b0-ee90b6ac2aee</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>jake45</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>7993d42b-bc7c-44e5-b6fa-7a8b2874c294</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>johndoe</t>
+  </si>
+  <si>
+    <t>27a23a50-e50d-45e4-bd9b-7227f48f6c00</t>
+  </si>
+  <si>
+    <t>Mary Lim</t>
+  </si>
+  <si>
+    <t>marlim</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>f1680687-8ee8-44a2-8fe2-058ed929403d</t>
   </si>
 </sst>
 </file>
@@ -568,12 +595,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -768,38 +795,95 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
@@ -810,24 +894,24 @@
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
@@ -838,8 +922,8 @@
       <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -850,8 +934,8 @@
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
@@ -859,19 +943,19 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
@@ -879,11 +963,11 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
@@ -894,8 +978,8 @@
       <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
@@ -903,11 +987,11 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
-      <c r="B39" s="1"/>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
@@ -915,19 +999,19 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="1"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
@@ -938,12 +1022,12 @@
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="3"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
@@ -954,8 +1038,8 @@
       <c r="B50" s="1"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="1"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
@@ -986,11 +1070,11 @@
       <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="3"/>
-      <c r="B59" s="1"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="8"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="3"/>
+      <c r="A60" s="1"/>
       <c r="B60" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -998,36 +1082,36 @@
       <c r="B61" s="1"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="7"/>
-      <c r="B62" s="8"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
+      <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="3"/>
-      <c r="B64" s="1"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
-      <c r="B65" s="2"/>
+      <c r="B65" s="1"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="1"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="1"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="1"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
@@ -1035,7 +1119,6 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
-      <c r="B71" s="1"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
@@ -1045,16 +1128,14 @@
       <c r="A73" s="3"/>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="3"/>
-      <c r="B75" s="1"/>
-    </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="3"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="2"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
@@ -1073,15 +1154,6 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="2"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>